<commit_message>
collision and overlap setup
</commit_message>
<xml_diff>
--- a/SpriteLibrary.xlsx
+++ b/SpriteLibrary.xlsx
@@ -45,15 +45,6 @@
     <t>info</t>
   </si>
   <si>
-    <t>single life</t>
-  </si>
-  <si>
-    <t>full life</t>
-  </si>
-  <si>
-    <t>invinceable</t>
-  </si>
-  <si>
     <t>orange</t>
   </si>
   <si>
@@ -358,6 +349,15 @@
   </si>
   <si>
     <t>DO NOT USE</t>
+  </si>
+  <si>
+    <t>single life crate</t>
+  </si>
+  <si>
+    <t>full life crate</t>
+  </si>
+  <si>
+    <t>invinceable crate</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +750,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -784,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,7 +792,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,13 +826,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,13 +840,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -854,13 +854,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -868,13 +868,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,13 +882,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -927,7 +927,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -941,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -984,10 +984,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>500</v>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,19 +1012,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
         <v>62</v>
-      </c>
-      <c r="F20" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C21">
         <v>100</v>
@@ -1041,10 +1041,10 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -1061,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23">
         <v>200</v>
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C24">
         <v>300</v>
@@ -1095,7 +1095,7 @@
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C25">
         <v>500</v>
@@ -1112,7 +1112,7 @@
         <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C26">
         <v>100</v>
@@ -1129,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C27">
         <v>200</v>
@@ -1146,7 +1146,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C28">
         <v>300</v>
@@ -1163,7 +1163,7 @@
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C29">
         <v>500</v>
@@ -1180,7 +1180,7 @@
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,10 +1188,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,13 +1199,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,13 +1213,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,13 +1227,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1241,10 +1241,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,10 +1252,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1263,10 +1263,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,10 +1274,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,10 +1285,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,10 +1296,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,7 +1307,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -1316,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -1333,7 +1333,7 @@
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C42">
         <v>100</v>
@@ -1350,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1367,7 +1367,7 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1384,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1401,7 +1401,7 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1409,7 +1409,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1418,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C47">
         <v>100</v>
@@ -1435,7 +1435,7 @@
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C48">
         <v>500</v>
@@ -1452,7 +1452,7 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C49">
         <v>500</v>
@@ -1469,7 +1469,7 @@
         <v>16</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -1486,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C51">
         <v>100</v>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,7 +1511,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C52">
         <v>100</v>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C53">
         <v>100</v>
@@ -1537,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,7 +1545,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>800</v>
@@ -1554,7 +1554,7 @@
         <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C55">
         <v>800</v>
@@ -1571,7 +1571,7 @@
         <v>16</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56">
         <v>800</v>
@@ -1588,10 +1588,10 @@
         <v>16</v>
       </c>
       <c r="E56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1599,7 +1599,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C57">
         <v>800</v>
@@ -1608,7 +1608,7 @@
         <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C58">
         <v>800</v>
@@ -1625,7 +1625,7 @@
         <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C59">
         <v>800</v>
@@ -1642,7 +1642,7 @@
         <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C60">
         <v>800</v>
@@ -1659,10 +1659,10 @@
         <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F60" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1670,7 +1670,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C61">
         <v>800</v>
@@ -1679,7 +1679,7 @@
         <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,7 +1687,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C62">
         <v>200</v>
@@ -1696,10 +1696,10 @@
         <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C63">
         <v>500</v>
@@ -1716,10 +1716,10 @@
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F63" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C64">
         <v>400</v>
@@ -1736,10 +1736,10 @@
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F64" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C65">
         <v>1000</v>
@@ -1756,10 +1756,10 @@
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,10 +1767,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,10 +1778,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F67" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,10 +1789,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1800,7 +1800,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,7 +1832,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sprite map parsing
</commit_message>
<xml_diff>
--- a/SpriteLibrary.xlsx
+++ b/SpriteLibrary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
   <si>
     <t>index</t>
   </si>
@@ -39,12 +39,6 @@
     <t>player</t>
   </si>
   <si>
-    <t>powerup</t>
-  </si>
-  <si>
-    <t>info</t>
-  </si>
-  <si>
     <t>orange</t>
   </si>
   <si>
@@ -210,9 +204,6 @@
     <t>gravity</t>
   </si>
   <si>
-    <t>shows dialogue when touching</t>
-  </si>
-  <si>
     <t>restores 10 health</t>
   </si>
   <si>
@@ -345,9 +336,6 @@
     <t>ceil generator single life</t>
   </si>
   <si>
-    <t>drops any life item DO NOT USE</t>
-  </si>
-  <si>
     <t>DO NOT USE</t>
   </si>
   <si>
@@ -358,6 +346,18 @@
   </si>
   <si>
     <t>invinceable crate</t>
+  </si>
+  <si>
+    <t>left laser</t>
+  </si>
+  <si>
+    <t>right laser</t>
+  </si>
+  <si>
+    <t>ceil laser</t>
+  </si>
+  <si>
+    <t>floor laser</t>
   </si>
 </sst>
 </file>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,22 +735,16 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -758,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -767,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -784,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -801,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,16 +803,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,13 +817,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,13 +831,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -854,13 +845,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -868,13 +859,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,10 +873,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>58</v>
@@ -896,16 +890,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13">
         <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -913,7 +904,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -927,13 +918,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,16 +935,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,13 +955,16 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,19 +972,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,16 +989,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>500</v>
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,19 +1009,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,19 +1029,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,13 +1046,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
@@ -1069,16 +1063,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,16 +1080,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D24">
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1103,16 +1097,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D25">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,13 +1114,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
@@ -1137,16 +1131,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,16 +1148,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C28">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,16 +1165,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29">
-        <v>500</v>
-      </c>
-      <c r="D29">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="F29" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,10 +1176,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,13 +1190,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,13 +1204,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,13 +1218,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1241,10 +1229,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1255,7 +1243,7 @@
         <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1263,10 +1251,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,10 +1262,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,10 +1273,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1296,10 +1284,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="C39">
+        <v>100</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,7 +1301,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -1316,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1324,7 +1318,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -1333,7 +1327,7 @@
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1335,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42">
         <v>100</v>
@@ -1350,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,7 +1352,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1367,7 +1361,7 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,7 +1369,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1384,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,7 +1386,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1401,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1409,7 +1403,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1418,7 +1412,7 @@
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,13 +1420,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C47">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -1443,7 +1437,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48">
         <v>500</v>
@@ -1452,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,16 +1454,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C49">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D49">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,7 +1471,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -1486,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,7 +1488,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>100</v>
@@ -1503,7 +1497,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,7 +1505,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52">
         <v>100</v>
@@ -1520,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,7 +1522,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="C53">
         <v>100</v>
@@ -1537,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,16 +1539,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C54">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="D54">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,16 +1556,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C55">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="D55">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,19 +1573,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C56">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1599,7 +1590,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C57">
         <v>800</v>
@@ -1608,7 +1599,7 @@
         <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1616,7 +1607,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C58">
         <v>800</v>
@@ -1625,7 +1616,7 @@
         <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1633,7 +1624,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C59">
         <v>800</v>
@@ -1642,7 +1633,10 @@
         <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1650,7 +1644,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C60">
         <v>800</v>
@@ -1659,10 +1653,7 @@
         <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1670,7 +1661,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C61">
         <v>800</v>
@@ -1679,7 +1670,7 @@
         <v>16</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,19 +1678,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="C62">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,19 +1695,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C63">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F63" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,19 +1715,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="C64">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="D64">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,19 +1732,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C65">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="D65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,10 +1752,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="C66">
+        <v>500</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,10 +1772,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="C67">
+        <v>400</v>
+      </c>
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
       </c>
       <c r="F67" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,10 +1792,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C68">
+        <v>1000</v>
+      </c>
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
       </c>
       <c r="F68" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1800,7 +1812,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="F69" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1808,7 +1823,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="F70" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1816,7 +1834,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="F71" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,7 +1845,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1832,7 +1853,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1861,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,7 +1869,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1877,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,7 +1885,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,11 +1893,35 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A78">
+  <sortState ref="A2:A82">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added bigbomb, small power bomb
</commit_message>
<xml_diff>
--- a/SpriteLibrary.xlsx
+++ b/SpriteLibrary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="116">
   <si>
     <t>index</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>floor laser</t>
+  </si>
+  <si>
+    <t>bomb, gravity NO USE</t>
+  </si>
+  <si>
+    <t>bomb NO USE</t>
   </si>
 </sst>
 </file>
@@ -698,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1007,7 @@
         <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed door performance, added blue door
</commit_message>
<xml_diff>
--- a/SpriteLibrary.xlsx
+++ b/SpriteLibrary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
   <si>
     <t>index</t>
   </si>
@@ -310,33 +310,6 @@
   </si>
   <si>
     <t>ceil tall building</t>
-  </si>
-  <si>
-    <t>floor generator robot</t>
-  </si>
-  <si>
-    <t>floor generator turret</t>
-  </si>
-  <si>
-    <t>floor generator brown block</t>
-  </si>
-  <si>
-    <t>ceil generator robot</t>
-  </si>
-  <si>
-    <t>ceil generator turret</t>
-  </si>
-  <si>
-    <t>ceil generator brown block</t>
-  </si>
-  <si>
-    <t>floor generator single life</t>
-  </si>
-  <si>
-    <t>ceil generator single life</t>
-  </si>
-  <si>
-    <t>DO NOT USE</t>
   </si>
   <si>
     <t>single life crate</t>
@@ -702,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -775,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -792,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -987,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,7 +980,7 @@
         <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1455,7 +1428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1472,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1489,7 +1462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1506,7 +1479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1523,12 +1496,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C53">
         <v>100</v>
@@ -1540,12 +1513,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C54">
         <v>100</v>
@@ -1557,12 +1530,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C55">
         <v>100</v>
@@ -1574,12 +1547,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C56">
         <v>100</v>
@@ -1591,13 +1564,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
-        <v>104</v>
-      </c>
       <c r="C57">
         <v>800</v>
       </c>
@@ -1608,13 +1578,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
-        <v>98</v>
-      </c>
       <c r="C58">
         <v>800</v>
       </c>
@@ -1625,13 +1592,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
-        <v>99</v>
-      </c>
       <c r="C59">
         <v>800</v>
       </c>
@@ -1641,17 +1605,11 @@
       <c r="E59" t="s">
         <v>9</v>
       </c>
-      <c r="F59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
       <c r="C60">
         <v>800</v>
       </c>
@@ -1662,13 +1620,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
-        <v>105</v>
-      </c>
       <c r="C61">
         <v>800</v>
       </c>
@@ -1679,13 +1634,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
-        <v>101</v>
-      </c>
       <c r="C62">
         <v>800</v>
       </c>
@@ -1696,13 +1648,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
       <c r="C63">
         <v>800</v>
       </c>
@@ -1712,17 +1661,11 @@
       <c r="E63" t="s">
         <v>9</v>
       </c>
-      <c r="F63" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
-        <v>103</v>
-      </c>
       <c r="C64">
         <v>800</v>
       </c>
@@ -1733,197 +1676,619 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
-        <v>35</v>
-      </c>
       <c r="C65">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
-      </c>
-      <c r="F65" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
-        <v>36</v>
-      </c>
       <c r="C66">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E66" t="s">
         <v>9</v>
       </c>
-      <c r="F66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
-        <v>37</v>
-      </c>
       <c r="C67">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="D67">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E67" t="s">
         <v>9</v>
       </c>
-      <c r="F67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
-        <v>38</v>
-      </c>
       <c r="C68">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="D68">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
-      </c>
-      <c r="F68" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
-        <v>39</v>
-      </c>
-      <c r="F69" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>800</v>
+      </c>
+      <c r="D69">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>800</v>
+      </c>
+      <c r="D70">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
-        <v>41</v>
-      </c>
-      <c r="F71" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>800</v>
+      </c>
+      <c r="D71">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>800</v>
+      </c>
+      <c r="D72">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>800</v>
+      </c>
+      <c r="D73">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>800</v>
+      </c>
+      <c r="D74">
+        <v>16</v>
+      </c>
+      <c r="E74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>800</v>
+      </c>
+      <c r="D75">
+        <v>16</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>800</v>
+      </c>
+      <c r="D76">
+        <v>16</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>800</v>
+      </c>
+      <c r="D77">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>800</v>
+      </c>
+      <c r="D78">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>800</v>
+      </c>
+      <c r="D79">
+        <v>16</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>800</v>
+      </c>
+      <c r="D80">
+        <v>16</v>
+      </c>
+      <c r="E80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81">
+        <v>800</v>
+      </c>
+      <c r="D81">
+        <v>16</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="C82">
+        <v>800</v>
+      </c>
+      <c r="D82">
+        <v>16</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="C83">
+        <v>800</v>
+      </c>
+      <c r="D83">
+        <v>16</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="C84">
+        <v>800</v>
+      </c>
+      <c r="D84">
+        <v>16</v>
+      </c>
+      <c r="E84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="C85">
+        <v>800</v>
+      </c>
+      <c r="D85">
+        <v>16</v>
+      </c>
+      <c r="E85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="C86">
+        <v>800</v>
+      </c>
+      <c r="D86">
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="C87">
+        <v>800</v>
+      </c>
+      <c r="D87">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="C88">
+        <v>800</v>
+      </c>
+      <c r="D88">
+        <v>16</v>
+      </c>
+      <c r="E88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>800</v>
+      </c>
+      <c r="D89">
+        <v>16</v>
+      </c>
+      <c r="E89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="C90">
+        <v>800</v>
+      </c>
+      <c r="D90">
+        <v>16</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="C91">
+        <v>800</v>
+      </c>
+      <c r="D91">
+        <v>16</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>800</v>
+      </c>
+      <c r="D92">
+        <v>16</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>35</v>
+      </c>
+      <c r="C93">
+        <v>200</v>
+      </c>
+      <c r="D93">
+        <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94">
+        <v>500</v>
+      </c>
+      <c r="D94">
+        <v>4</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95">
+        <v>400</v>
+      </c>
+      <c r="D95">
+        <v>6</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96">
+        <v>1000</v>
+      </c>
+      <c r="D96">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>39</v>
+      </c>
+      <c r="F97" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="F98" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>41</v>
+      </c>
+      <c r="F99" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>42</v>
+      </c>
+      <c r="C100">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>43</v>
+      </c>
+      <c r="C101">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>44</v>
+      </c>
+      <c r="C102">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C103">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>49</v>
+      </c>
+      <c r="C107">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
         <v>51</v>
+      </c>
+      <c r="C109">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>